<commit_message>
reports dir filled with content
</commit_message>
<xml_diff>
--- a/chapter03/reports/darwin_notInRuleset_2.xlsx
+++ b/chapter03/reports/darwin_notInRuleset_2.xlsx
@@ -17,16 +17,22 @@
     <t>id</t>
   </si>
   <si>
-    <t>dest_ip_start_int</t>
+    <t>rule_number</t>
+  </si>
+  <si>
+    <t>rule_name</t>
+  </si>
+  <si>
+    <t>dest_ip_start</t>
+  </si>
+  <si>
+    <t>dest_ip_end</t>
   </si>
   <si>
     <t>dest_ip_end_int</t>
   </si>
   <si>
-    <t>dest_ip_type</t>
-  </si>
-  <si>
-    <t>dest_ip_start</t>
+    <t>dest_ip_start_int</t>
   </si>
   <si>
     <t>dest_ip_cidr</t>
@@ -35,16 +41,13 @@
     <t>json_services</t>
   </si>
   <si>
-    <t>rule_name</t>
+    <t>dest_ip_type</t>
   </si>
   <si>
-    <t>rule_number</t>
+    <t>373</t>
   </si>
   <si>
-    <t>dest_ip_end</t>
-  </si>
-  <si>
-    <t>host</t>
+    <t>e_SAP_ERP_S4P</t>
   </si>
   <si>
     <t>139.25.227.144</t>
@@ -53,10 +56,7 @@
     <t>["443/tcp"]</t>
   </si>
   <si>
-    <t>e_SAP_ERP_S4P</t>
-  </si>
-  <si>
-    <t>373</t>
+    <t>host</t>
   </si>
 </sst>
 </file>
@@ -143,32 +143,32 @@
       <c r="A2" t="n">
         <v>1271.0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
         <v>2.33372968E9</v>
       </c>
-      <c r="C2" t="n">
+      <c r="G2" t="n">
         <v>2.33372968E9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>32.0</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>